<commit_message>
Iteration Plan 2 complete
</commit_message>
<xml_diff>
--- a/Iteration_Plan/Iteration Plan_Agile Backlog and Release Summary_Group2.xlsx
+++ b/Iteration_Plan/Iteration Plan_Agile Backlog and Release Summary_Group2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Final Project\FinalProject\Iteration_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E91FDDA-A63D-43F0-8600-2531D232848A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10D7FF9-78DA-4B6E-9591-C38E8A041251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22248" windowHeight="13176" activeTab="1" xr2:uid="{4F8364D9-F33F-4911-8F06-4075FAA056D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{4F8364D9-F33F-4911-8F06-4075FAA056D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 Plan" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="112">
   <si>
     <t>Project</t>
   </si>
@@ -530,9 +530,6 @@
     <t>Design: Calendar Page</t>
   </si>
   <si>
-    <t>AAA: Refine</t>
-  </si>
-  <si>
     <t>BY, JA, RZ</t>
   </si>
   <si>
@@ -576,6 +573,36 @@
   </si>
   <si>
     <t>New solution</t>
+  </si>
+  <si>
+    <t>UC02-04: Task CRUD operations - Refine</t>
+  </si>
+  <si>
+    <t>UC06: Tasks are categorized and showed as expected - Refine</t>
+  </si>
+  <si>
+    <t>Website Design: Color Plan, Style, Logo, etc.</t>
+  </si>
+  <si>
+    <t>Bootstrap study &amp; integration</t>
+  </si>
+  <si>
+    <t>Views: Webpage refine</t>
+  </si>
+  <si>
+    <t>Dynamic Timetable view Implementation</t>
+  </si>
+  <si>
+    <t>View: Home Page Task Chart and Pie Chart implementation</t>
+  </si>
+  <si>
+    <t>Feature: Small ChatGPT add-on feature that provides plan to finish tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual Studio </t>
+  </si>
+  <si>
+    <t>Finish inception documents</t>
   </si>
 </sst>
 </file>
@@ -697,7 +724,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,6 +806,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -889,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1073,6 +1112,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1137,10 +1177,55 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,9 +1762,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1717,7 +1802,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1823,7 +1908,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1965,7 +2050,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1978,8 +2063,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2023,34 +2108,34 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="78"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="11" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
@@ -2071,7 +2156,7 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>69</v>
@@ -2083,7 +2168,7 @@
         <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>69</v>
@@ -2098,7 +2183,7 @@
         <v>82</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -2110,7 +2195,7 @@
         <v>83</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="18"/>
     </row>
@@ -2119,10 +2204,10 @@
         <v>105</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="18"/>
     </row>
@@ -2131,10 +2216,10 @@
         <v>106</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="18"/>
     </row>
@@ -2143,10 +2228,10 @@
         <v>107</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" s="18"/>
     </row>
@@ -2155,10 +2240,10 @@
         <v>108</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="18"/>
     </row>
@@ -2166,11 +2251,11 @@
       <c r="A20" s="19">
         <v>109</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="71"/>
@@ -2180,10 +2265,10 @@
         <v>110</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="18"/>
     </row>
@@ -2194,13 +2279,13 @@
       <c r="D22" s="18"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
@@ -2218,7 +2303,7 @@
         <v>75</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>70</v>
@@ -2229,7 +2314,7 @@
         <v>76</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>70</v>
@@ -2240,7 +2325,7 @@
         <v>77</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>70</v>
@@ -2251,7 +2336,7 @@
         <v>74</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>70</v>
@@ -2262,7 +2347,7 @@
         <v>78</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>70</v>
@@ -2273,7 +2358,7 @@
         <v>79</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>70</v>
@@ -2284,7 +2369,7 @@
         <v>80</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>70</v>
@@ -2295,7 +2380,7 @@
         <v>84</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>70</v>
@@ -2306,7 +2391,7 @@
         <v>85</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>70</v>
@@ -2373,8 +2458,8 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J13"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2390,150 +2475,150 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
     </row>
     <row r="10" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
     </row>
     <row r="13" spans="1:10" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
@@ -2566,14 +2651,14 @@
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
-      <c r="E17" s="98"/>
+      <c r="E17" s="75"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="72">
         <v>1</v>
@@ -2581,14 +2666,14 @@
       <c r="D18" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="98"/>
+      <c r="E18" s="75"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>102</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="10">
         <v>1</v>
@@ -2596,7 +2681,7 @@
       <c r="D19" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="98"/>
+      <c r="E19" s="75"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
@@ -2609,7 +2694,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2623,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2631,13 +2716,13 @@
         <v>105</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="72">
         <v>2</v>
       </c>
       <c r="D22" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2645,13 +2730,13 @@
         <v>106</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="10">
         <v>4</v>
       </c>
       <c r="D23" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2659,13 +2744,13 @@
         <v>107</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="21">
         <v>2</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2673,27 +2758,27 @@
         <v>108</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="21">
         <v>1</v>
       </c>
       <c r="D25" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>109</v>
       </c>
-      <c r="B26" s="97" t="s">
-        <v>95</v>
+      <c r="B26" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="C26" s="21">
         <v>1</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2701,13 +2786,13 @@
         <v>110</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="21">
         <v>1</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2752,19 +2837,19 @@
       <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="81"/>
       <c r="B34" s="22"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="80"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="22"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="80"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="22"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -2805,11 +2890,11 @@
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="81" t="s">
+      <c r="E43" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
@@ -2818,31 +2903,31 @@
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="20"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="33"/>
@@ -2888,14 +2973,14 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G12"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.5546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
@@ -2910,105 +2995,105 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
     </row>
     <row r="11" spans="1:7" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
     </row>
     <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
@@ -3033,10 +3118,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -3056,8 +3141,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="17" t="s">
         <v>23</v>
       </c>
@@ -3075,100 +3160,166 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
+      <c r="A18" s="99">
+        <v>1</v>
+      </c>
+      <c r="B18" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="101">
+        <v>6</v>
+      </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="24"/>
+      <c r="A19" s="102">
+        <v>101</v>
+      </c>
+      <c r="B19" s="103" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110">
+        <v>1</v>
+      </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="24"/>
+      <c r="A20" s="102">
+        <v>102</v>
+      </c>
+      <c r="B20" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="104">
+        <v>1</v>
+      </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="24"/>
+      <c r="A21" s="102">
+        <v>103</v>
+      </c>
+      <c r="B21" s="105" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109">
+        <v>2</v>
+      </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="24"/>
+      <c r="A22" s="102">
+        <v>104</v>
+      </c>
+      <c r="B22" s="105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109">
+        <v>2</v>
+      </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="24"/>
+      <c r="A23" s="102">
+        <v>105</v>
+      </c>
+      <c r="B23" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="109"/>
+      <c r="D23" s="110">
+        <v>2</v>
+      </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="24"/>
+      <c r="A24" s="102">
+        <v>106</v>
+      </c>
+      <c r="B24" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="109"/>
+      <c r="D24" s="104">
+        <v>4</v>
+      </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="24"/>
+      <c r="A25" s="102">
+        <v>107</v>
+      </c>
+      <c r="B25" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109">
+        <v>2</v>
+      </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="54"/>
+      <c r="A26" s="102">
+        <v>108</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="104"/>
+      <c r="D26" s="109">
+        <v>1</v>
+      </c>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="54"/>
+      <c r="A27" s="102">
+        <v>109</v>
+      </c>
+      <c r="B27" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="104"/>
+      <c r="D27" s="109">
+        <v>1</v>
+      </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="54"/>
+      <c r="A28" s="102">
+        <v>110</v>
+      </c>
+      <c r="B28" s="105" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="104"/>
+      <c r="D28" s="109">
+        <v>1</v>
+      </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
@@ -3382,53 +3533,53 @@
       <c r="H51" s="26"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="92" t="s">
+      <c r="A52" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="93"/>
-      <c r="C52" s="94" cm="1">
+      <c r="B52" s="94"/>
+      <c r="C52" s="95" cm="1">
         <f t="array" ref="C52">SUM(C18:C51*4)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="94" cm="1">
+        <v>24</v>
+      </c>
+      <c r="D52" s="95" cm="1">
         <f t="array" ref="D52">SUM(D18:D51*4)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="94" cm="1">
+        <v>68</v>
+      </c>
+      <c r="E52" s="95" cm="1">
         <f t="array" ref="E52">SUM(E18:E51*4)</f>
         <v>0</v>
       </c>
-      <c r="F52" s="94" cm="1">
+      <c r="F52" s="95" cm="1">
         <f t="array" ref="F52">SUM(F18:F51*4)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="94" cm="1">
+      <c r="G52" s="95" cm="1">
         <f t="array" ref="G52">SUM(G18:G51*4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="93"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="95"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="85" t="s">
+      <c r="A54" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="86"/>
-      <c r="C54" s="87">
+      <c r="B54" s="87"/>
+      <c r="C54" s="88">
         <f>SUM(C52:G53)</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="89"/>
+        <v>92</v>
+      </c>
+      <c r="D54" s="89"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3456,14 +3607,14 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
@@ -3495,34 +3646,34 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="78"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="11" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
@@ -3539,61 +3690,121 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="19">
+        <v>201</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="19">
+        <v>202</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="19">
+        <v>203</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="19">
+        <v>204</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="19">
+        <v>205</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="19">
+        <v>206</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="19">
+        <v>207</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="19">
+        <v>208</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D19" s="10"/>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>209</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="10"/>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
@@ -3607,49 +3818,103 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="A26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="A28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
+      <c r="A29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="A30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="A31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+      <c r="A33" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
@@ -3674,8 +3939,12 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
@@ -3686,11 +3955,11 @@
       <c r="B40" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="75"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -3720,8 +3989,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3736,150 +4005,150 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
     </row>
     <row r="10" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
     </row>
     <row r="13" spans="1:10" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
@@ -3914,58 +4183,130 @@
       <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="19">
+        <v>201</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="19"/>
+      <c r="A19" s="19">
+        <v>202</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="21">
+        <v>3</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="19">
+        <v>203</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="21">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="19"/>
+      <c r="A21" s="19">
+        <v>204</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="19">
+        <v>205</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="21">
+        <v>3</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="19"/>
+      <c r="A23" s="19">
+        <v>206</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="21">
+        <v>3</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="19"/>
+      <c r="A24" s="19">
+        <v>207</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="21">
+        <v>4</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="19">
+        <v>208</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="21">
+        <v>4</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="19"/>
+      <c r="A26" s="19">
+        <v>209</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="21">
+        <v>2</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
@@ -3993,9 +4334,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
-      <c r="B31" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="23"/>
     </row>
@@ -4069,23 +4408,23 @@
       <c r="B43" s="47"/>
       <c r="C43" s="47"/>
       <c r="D43" s="46"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="20"/>
       <c r="C44" s="21"/>
       <c r="D44" s="20"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
@@ -4094,15 +4433,23 @@
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="A47" s="23">
+        <v>221</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="10">
+        <v>4</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
@@ -4165,14 +4512,14 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="84.44140625" style="16" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
@@ -4187,105 +4534,105 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="1:7" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
     </row>
     <row r="11" spans="1:7" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
     </row>
     <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
@@ -4310,10 +4657,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -4333,8 +4680,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="17" t="s">
         <v>23</v>
       </c>
@@ -4352,182 +4699,302 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
+      <c r="A18" s="99">
+        <v>1</v>
+      </c>
+      <c r="B18" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="101">
+        <v>6</v>
+      </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="24"/>
+      <c r="A19" s="102">
+        <v>101</v>
+      </c>
+      <c r="B19" s="103" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110">
+        <v>1</v>
+      </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="24"/>
+      <c r="A20" s="102">
+        <v>102</v>
+      </c>
+      <c r="B20" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="104">
+        <v>1</v>
+      </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="24"/>
+      <c r="A21" s="102">
+        <v>103</v>
+      </c>
+      <c r="B21" s="105" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109">
+        <v>2</v>
+      </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="24"/>
+      <c r="A22" s="102">
+        <v>104</v>
+      </c>
+      <c r="B22" s="105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109">
+        <v>2</v>
+      </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="24"/>
+      <c r="A23" s="102">
+        <v>105</v>
+      </c>
+      <c r="B23" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="109"/>
+      <c r="D23" s="110">
+        <v>2</v>
+      </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="24"/>
+      <c r="A24" s="102">
+        <v>106</v>
+      </c>
+      <c r="B24" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="109"/>
+      <c r="D24" s="104">
+        <v>4</v>
+      </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="24"/>
+      <c r="A25" s="102">
+        <v>107</v>
+      </c>
+      <c r="B25" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109">
+        <v>2</v>
+      </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="54"/>
+      <c r="A26" s="102">
+        <v>108</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="104"/>
+      <c r="D26" s="109">
+        <v>1</v>
+      </c>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="54"/>
+      <c r="A27" s="102">
+        <v>109</v>
+      </c>
+      <c r="B27" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="104"/>
+      <c r="D27" s="109">
+        <v>1</v>
+      </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="54"/>
+      <c r="A28" s="102">
+        <v>110</v>
+      </c>
+      <c r="B28" s="105" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="104"/>
+      <c r="D28" s="109">
+        <v>1</v>
+      </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="24"/>
+      <c r="A29" s="111">
+        <v>201</v>
+      </c>
+      <c r="B29" s="112" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="113"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114">
+        <v>2</v>
+      </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="24"/>
+      <c r="A30" s="111">
+        <v>202</v>
+      </c>
+      <c r="B30" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="113"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="114">
+        <v>3</v>
+      </c>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="24"/>
+      <c r="A31" s="111">
+        <v>203</v>
+      </c>
+      <c r="B31" s="112" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="113"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114">
+        <v>1</v>
+      </c>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="24"/>
+      <c r="A32" s="111">
+        <v>204</v>
+      </c>
+      <c r="B32" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="113"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114">
+        <v>1</v>
+      </c>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="24"/>
+      <c r="A33" s="111">
+        <v>205</v>
+      </c>
+      <c r="B33" s="115" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="113"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114">
+        <v>3</v>
+      </c>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="24"/>
+      <c r="A34" s="111">
+        <v>206</v>
+      </c>
+      <c r="B34" s="115" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="113"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="114">
+        <v>3</v>
+      </c>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="24"/>
+      <c r="A35" s="111">
+        <v>207</v>
+      </c>
+      <c r="B35" s="115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="113"/>
+      <c r="D35" s="114"/>
+      <c r="E35" s="114">
+        <v>4</v>
+      </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="52"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="24"/>
+      <c r="A36" s="111">
+        <v>208</v>
+      </c>
+      <c r="B36" s="115" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="113"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114">
+        <v>4</v>
+      </c>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
+      <c r="A37" s="111">
+        <v>209</v>
+      </c>
+      <c r="B37" s="112" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="116"/>
+      <c r="D37" s="116"/>
+      <c r="E37" s="114">
+        <v>2</v>
+      </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
     </row>
@@ -4668,53 +5135,53 @@
       <c r="H52" s="26"/>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="92" t="s">
+      <c r="A53" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="92"/>
-      <c r="C53" s="94" cm="1">
+      <c r="B53" s="93"/>
+      <c r="C53" s="95" cm="1">
         <f t="array" ref="C53">SUM(C18:C52*4)</f>
-        <v>0</v>
-      </c>
-      <c r="D53" s="94" cm="1">
+        <v>24</v>
+      </c>
+      <c r="D53" s="95" cm="1">
         <f t="array" ref="D53">SUM(D18:D52*4)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="94" cm="1">
+        <v>68</v>
+      </c>
+      <c r="E53" s="95" cm="1">
         <f t="array" ref="E53">SUM(E18:E52*4)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="94" cm="1">
+        <v>92</v>
+      </c>
+      <c r="F53" s="95" cm="1">
         <f t="array" ref="F53">SUM(F18:F52*4)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="94" cm="1">
+      <c r="G53" s="95" cm="1">
         <f t="array" ref="G53">SUM(G18:G52*4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="92"/>
-      <c r="B54" s="92"/>
-      <c r="C54" s="94"/>
-      <c r="D54" s="94"/>
-      <c r="E54" s="94"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="94"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="95" t="s">
+      <c r="A55" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="95"/>
-      <c r="C55" s="96">
+      <c r="B55" s="96"/>
+      <c r="C55" s="97">
         <f>SUM(C53:G54)</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="96"/>
-      <c r="E55" s="96"/>
-      <c r="F55" s="96"/>
-      <c r="G55" s="96"/>
+        <v>184</v>
+      </c>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4781,34 +5248,34 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="78"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="11" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
@@ -4873,13 +5340,13 @@
       <c r="D19" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="40" t="s">
@@ -4972,11 +5439,11 @@
       <c r="B40" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="75"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -5022,150 +5489,150 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
     </row>
     <row r="13" spans="1:10" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
@@ -5353,68 +5820,68 @@
       <c r="B43" s="47"/>
       <c r="C43" s="47"/>
       <c r="D43" s="46"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="20"/>
       <c r="C44" s="50"/>
       <c r="D44" s="51"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="47"/>
       <c r="C45" s="21"/>
       <c r="D45" s="51"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="47"/>
       <c r="C46" s="21"/>
       <c r="D46" s="51"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="47"/>
       <c r="C47" s="21"/>
       <c r="D47" s="51"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="83"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="47"/>
       <c r="C48" s="21"/>
       <c r="D48" s="51"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="42"/>
       <c r="B49" s="43"/>
       <c r="C49" s="44"/>
       <c r="D49" s="43"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
@@ -5423,9 +5890,9 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="23"/>
@@ -5516,105 +5983,105 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="1:7" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
     </row>
     <row r="11" spans="1:7" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
     </row>
     <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
@@ -5639,10 +6106,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -5662,8 +6129,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="17" t="s">
         <v>23</v>
       </c>
@@ -6024,53 +6491,53 @@
       <c r="H55" s="26"/>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="92" t="s">
+      <c r="A56" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="92"/>
-      <c r="C56" s="94" cm="1">
+      <c r="B56" s="93"/>
+      <c r="C56" s="95" cm="1">
         <f t="array" ref="C56">SUM(C18:C55*4)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="94" cm="1">
+      <c r="D56" s="95" cm="1">
         <f t="array" ref="D56">SUM(D18:D55*4)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="94" cm="1">
+      <c r="E56" s="95" cm="1">
         <f t="array" ref="E56">SUM(E18:E55*4)</f>
         <v>0</v>
       </c>
-      <c r="F56" s="94" cm="1">
+      <c r="F56" s="95" cm="1">
         <f t="array" ref="F56">SUM(F18:F55*4)</f>
         <v>0</v>
       </c>
-      <c r="G56" s="94" cm="1">
+      <c r="G56" s="95" cm="1">
         <f t="array" ref="G56">SUM(G18:G55*4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="92"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="94"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="94"/>
-      <c r="F57" s="94"/>
-      <c r="G57" s="94"/>
+      <c r="A57" s="93"/>
+      <c r="B57" s="93"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="95"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="95"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="95" t="s">
+      <c r="A58" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="95"/>
-      <c r="C58" s="96">
+      <c r="B58" s="96"/>
+      <c r="C58" s="97">
         <f>SUM(C56:G57)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="96"/>
-      <c r="E58" s="96"/>
-      <c r="F58" s="96"/>
-      <c r="G58" s="96"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6091,26 +6558,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65b9d225-16ca-46f6-ae18-b6551cf021c0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010026FD05EB56FECE40B429A2882E76EFBE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0b42309774119f5dcc422c245407344">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4" xmlns:ns3="65b9d225-16ca-46f6-ae18-b6551cf021c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9aa116f817a62313d8a59877ac597812" ns2:_="" ns3:_="">
     <xsd:import namespace="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4"/>
@@ -6313,26 +6760,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BC56548-19A4-4C90-9137-2F7841029EC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4"/>
-    <ds:schemaRef ds:uri="65b9d225-16ca-46f6-ae18-b6551cf021c0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE6DBF0-6AD3-41C7-9516-5FD4B9A4B9B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65b9d225-16ca-46f6-ae18-b6551cf021c0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74693F4-D0C0-4387-8062-352395039D6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6349,4 +6797,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE6DBF0-6AD3-41C7-9516-5FD4B9A4B9B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BC56548-19A4-4C90-9137-2F7841029EC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1e7187b-45d7-4b0b-bba7-dc63b8bbb5b4"/>
+    <ds:schemaRef ds:uri="65b9d225-16ca-46f6-ae18-b6551cf021c0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>